<commit_message>
update core auto run api to complete case Onboarding
</commit_message>
<xml_diff>
--- a/src/test/resources/Onboarding.xlsx
+++ b/src/test/resources/Onboarding.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="794">
   <si>
     <t>id</t>
   </si>
@@ -3146,6 +3146,36 @@
   </si>
   <si>
     <t>CA-KWMAIMDW</t>
+  </si>
+  <si>
+    <t>CA-R7GIFD1J</t>
+  </si>
+  <si>
+    <t>CA-O2MQ94QD</t>
+  </si>
+  <si>
+    <t>CA-S78DHH83</t>
+  </si>
+  <si>
+    <t>CA-CFUNBSAW</t>
+  </si>
+  <si>
+    <t>CA-M8PQ6KU6</t>
+  </si>
+  <si>
+    <t>CA-DJXJYTFJ</t>
+  </si>
+  <si>
+    <t>CA-JQPBNPRT</t>
+  </si>
+  <si>
+    <t>CA-GZRTBNIG</t>
+  </si>
+  <si>
+    <t>CA-RWG34YF3</t>
+  </si>
+  <si>
+    <t>CA-5VQT5TDJ</t>
   </si>
 </sst>
 </file>
@@ -3901,7 +3931,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>783</v>
+        <v>793</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>779</v>

</xml_diff>